<commit_message>
finished problem updated in console view
</commit_message>
<xml_diff>
--- a/src/main/resources/marks xlsheet.xlsx
+++ b/src/main/resources/marks xlsheet.xlsx
@@ -116,7 +116,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -126,10 +126,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -153,10 +149,10 @@
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22:A41"/>
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.54"/>
   </cols>
@@ -165,7 +161,7 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -192,7 +188,7 @@
       <c r="B4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="M4" s="3"/>
+      <c r="M4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">

</xml_diff>